<commit_message>
Actualizacion interfaz vida estudiantil
Se actualiza los requerimientos según la solicitud final
</commit_message>
<xml_diff>
--- a/documentacion/vidaestudiantil/Subida a Educatico/ficha_educatico-AGENDAESTUDIANTL.xlsx
+++ b/documentacion/vidaestudiantil/Subida a Educatico/ficha_educatico-AGENDAESTUDIANTL.xlsx
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="307">
   <si>
     <t>Título</t>
   </si>
@@ -1499,6 +1499,33 @@
     <t xml:space="preserve">
 Adjunto: folleto propuesta metodologica teatro en el aula 2020 web.pdf
 </t>
+  </si>
+  <si>
+    <t>ENLACE LISTO</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/servicio-comunal</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/aulas-escucha</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/erase-vez</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/teatro-aula</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/ruta-museos</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/gobierno-estudiantil</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/programa-convivir</t>
+  </si>
+  <si>
+    <t>https://www.mep.go.cr/educatico/educar-sostenibilidad-bandera-azul-ecologica</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1784,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1876,12 +1903,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1930,6 +1951,24 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1939,9 +1978,45 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1954,59 +2029,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2106,7 +2148,7 @@
       <xdr:rowOff>511970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>663076</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>532679</xdr:rowOff>
@@ -2139,15 +2181,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>1447023</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>149242</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1425064</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>549699</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>118332</xdr:rowOff>
+      <xdr:rowOff>261938</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2164,8 +2206,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8477250" y="21854336"/>
-          <a:ext cx="3127658" cy="1755027"/>
+          <a:off x="8512969" y="22509180"/>
+          <a:ext cx="2216574" cy="1243789"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2178,12 +2220,12 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>35719</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>238126</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1194086</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>267558</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>88460</xdr:rowOff>
     </xdr:to>
@@ -2202,8 +2244,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8501063" y="17728407"/>
-          <a:ext cx="2872867" cy="1624366"/>
+          <a:off x="8501063" y="18252281"/>
+          <a:ext cx="1946339" cy="1100492"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2220,8 +2262,8 @@
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>82530</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1654968</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>132620</xdr:rowOff>
     </xdr:to>
@@ -2241,7 +2283,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8515100" y="7453312"/>
-          <a:ext cx="1747274" cy="977964"/>
+          <a:ext cx="1605212" cy="977964"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2280,6 +2322,44 @@
         <a:xfrm>
           <a:off x="8477251" y="3865066"/>
           <a:ext cx="1631156" cy="897433"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1678905</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>128083</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8512969" y="9691687"/>
+          <a:ext cx="1631280" cy="1032959"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2580,8 +2660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:A53"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2593,31 +2673,32 @@
     <col min="10" max="10" width="20.7109375" style="31" customWidth="1"/>
     <col min="11" max="11" width="20" style="31" customWidth="1"/>
     <col min="12" max="12" width="40.85546875" style="31" customWidth="1"/>
-    <col min="13" max="14" width="25.7109375" style="31" customWidth="1"/>
-    <col min="15" max="16" width="20.7109375" style="31" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" style="31" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" style="31" hidden="1" customWidth="1"/>
+    <col min="15" max="16" width="20.7109375" style="31" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="25.7109375" style="39" customWidth="1"/>
     <col min="18" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="78" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
       <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="1:18" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2669,6 +2750,9 @@
       <c r="P2" s="27" t="s">
         <v>6</v>
       </c>
+      <c r="Q2" s="82" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="3" spans="1:18" ht="186.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
@@ -2683,7 +2767,7 @@
       <c r="D3" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="46" t="s">
         <v>255</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -2692,7 +2776,7 @@
       <c r="G3" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="45" t="s">
         <v>252</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -2707,7 +2791,7 @@
       <c r="L3" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="51" t="s">
         <v>285</v>
       </c>
       <c r="N3" s="5" t="s">
@@ -2715,614 +2799,620 @@
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="6"/>
+      <c r="Q3" s="86" t="s">
+        <v>299</v>
+      </c>
       <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="81" t="s">
         <v>278</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="H4" s="66" t="s">
+      <c r="H4" s="73" t="s">
         <v>252</v>
       </c>
-      <c r="I4" s="66" t="s">
+      <c r="I4" s="73" t="s">
         <v>256</v>
       </c>
-      <c r="J4" s="66" t="s">
+      <c r="J4" s="73" t="s">
         <v>259</v>
       </c>
-      <c r="K4" s="66" t="s">
+      <c r="K4" s="73" t="s">
         <v>260</v>
       </c>
       <c r="L4" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="74" t="s">
+      <c r="M4" s="70" t="s">
         <v>285</v>
       </c>
-      <c r="N4" s="66" t="s">
+      <c r="N4" s="73" t="s">
         <v>288</v>
       </c>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="6"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="83" t="s">
+        <v>299</v>
+      </c>
       <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
       <c r="L5" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="M5" s="75"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="6"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="84"/>
       <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
       <c r="L6" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="M6" s="75"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="6"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="84"/>
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
       <c r="L7" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="M7" s="75"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="6"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="84"/>
       <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="65"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
       <c r="L8" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="M8" s="75"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="6"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="84"/>
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
       <c r="L9" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="M9" s="75"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="6"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="84"/>
       <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
       <c r="L10" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="M10" s="75"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="6"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="84"/>
       <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="65"/>
+      <c r="A11" s="81"/>
       <c r="B11" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
       <c r="L11" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="M11" s="75"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="6"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="84"/>
       <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="65"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
       <c r="L12" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="M12" s="76"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="6"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="75"/>
+      <c r="Q12" s="85"/>
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="81" t="s">
         <v>276</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="H13" s="58" t="s">
+      <c r="H13" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="62" t="s">
         <v>259</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="62" t="s">
         <v>260</v>
       </c>
       <c r="L13" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="M13" s="77" t="s">
+      <c r="M13" s="65" t="s">
         <v>285</v>
       </c>
-      <c r="N13" s="58" t="s">
+      <c r="N13" s="62" t="s">
         <v>289</v>
       </c>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="6"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="83" t="s">
+        <v>300</v>
+      </c>
       <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="65"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
       <c r="L14" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="M14" s="78"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="6"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="84"/>
       <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="65"/>
+      <c r="A15" s="81"/>
       <c r="B15" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
       <c r="L15" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="M15" s="78"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="6"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="84"/>
       <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="65"/>
+      <c r="A16" s="81"/>
       <c r="B16" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
       <c r="L16" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="M16" s="78"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="6"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="84"/>
       <c r="R16" s="6"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="65"/>
+      <c r="A17" s="81"/>
       <c r="B17" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
       <c r="L17" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="M17" s="78"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="6"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="84"/>
       <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="65"/>
+      <c r="A18" s="81"/>
       <c r="B18" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
       <c r="L18" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="M18" s="78"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="6"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="84"/>
       <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="65"/>
+      <c r="A19" s="81"/>
       <c r="B19" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
       <c r="L19" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="M19" s="78"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="6"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="84"/>
       <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="65"/>
+      <c r="A20" s="81"/>
       <c r="B20" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
       <c r="L20" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="M20" s="78"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="6"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="85"/>
       <c r="R20" s="6"/>
     </row>
     <row r="21" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="81" t="s">
         <v>275</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="68" t="s">
         <v>251</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="68" t="s">
         <v>286</v>
       </c>
-      <c r="E21" s="61" t="s">
+      <c r="E21" s="68" t="s">
         <v>255</v>
       </c>
-      <c r="F21" s="61" t="s">
+      <c r="F21" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="68" t="s">
         <v>254</v>
       </c>
-      <c r="H21" s="61" t="s">
+      <c r="H21" s="68" t="s">
         <v>252</v>
       </c>
-      <c r="I21" s="61" t="s">
+      <c r="I21" s="68" t="s">
         <v>256</v>
       </c>
-      <c r="J21" s="61" t="s">
+      <c r="J21" s="68" t="s">
         <v>259</v>
       </c>
-      <c r="K21" s="61" t="s">
+      <c r="K21" s="68" t="s">
         <v>260</v>
       </c>
       <c r="L21" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="M21" s="79" t="s">
-        <v>285</v>
-      </c>
-      <c r="N21" s="61" t="s">
+      <c r="M21" s="69"/>
+      <c r="N21" s="68" t="s">
         <v>290</v>
       </c>
-      <c r="O21" s="61"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="6"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="68"/>
+      <c r="Q21" s="83" t="s">
+        <v>301</v>
+      </c>
       <c r="R21" s="6"/>
     </row>
     <row r="22" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="65"/>
+      <c r="A22" s="81"/>
       <c r="B22" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="68"/>
       <c r="L22" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="M22" s="79"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="6"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="68"/>
+      <c r="P22" s="68"/>
+      <c r="Q22" s="84"/>
       <c r="R22" s="6"/>
     </row>
     <row r="23" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="65"/>
+      <c r="A23" s="81"/>
       <c r="B23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="68"/>
       <c r="L23" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="M23" s="79"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="6"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="68"/>
+      <c r="O23" s="68"/>
+      <c r="P23" s="68"/>
+      <c r="Q23" s="84"/>
       <c r="R23" s="6"/>
     </row>
     <row r="24" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="65"/>
+      <c r="A24" s="81"/>
       <c r="B24" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
       <c r="L24" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="M24" s="79"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="6"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="68"/>
+      <c r="Q24" s="84"/>
       <c r="R24" s="6"/>
     </row>
     <row r="25" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="65"/>
+      <c r="A25" s="81"/>
       <c r="B25" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="68"/>
       <c r="L25" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="M25" s="79"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="40"/>
+      <c r="M25" s="69"/>
+      <c r="N25" s="68"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="68"/>
+      <c r="Q25" s="85"/>
       <c r="R25" s="6"/>
     </row>
     <row r="26" spans="1:18" ht="244.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="44" t="s">
         <v>203</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -3355,7 +3445,7 @@
       <c r="L26" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="M26" s="53" t="s">
+      <c r="M26" s="51" t="s">
         <v>285</v>
       </c>
       <c r="N26" s="5" t="s">
@@ -3363,7 +3453,9 @@
       </c>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-      <c r="Q26" s="41"/>
+      <c r="Q26" s="86" t="s">
+        <v>302</v>
+      </c>
       <c r="R26" s="6"/>
     </row>
     <row r="27" spans="1:18" ht="255" x14ac:dyDescent="0.2">
@@ -3403,7 +3495,7 @@
       <c r="L27" s="35" t="s">
         <v>296</v>
       </c>
-      <c r="M27" s="54" t="s">
+      <c r="M27" s="52" t="s">
         <v>285</v>
       </c>
       <c r="N27" s="34" t="s">
@@ -3411,696 +3503,704 @@
       </c>
       <c r="O27" s="34"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="41"/>
+      <c r="Q27" s="86" t="s">
+        <v>303</v>
+      </c>
       <c r="R27" s="6"/>
     </row>
     <row r="28" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="76" t="s">
         <v>274</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58" t="s">
+      <c r="E28" s="62"/>
+      <c r="F28" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="G28" s="58" t="s">
+      <c r="G28" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="H28" s="58" t="s">
+      <c r="H28" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="I28" s="58" t="s">
+      <c r="I28" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
       <c r="L28" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="M28" s="77"/>
-      <c r="N28" s="58" t="s">
+      <c r="M28" s="65"/>
+      <c r="N28" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="41"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="83" t="s">
+        <v>304</v>
+      </c>
       <c r="R28" s="6"/>
     </row>
     <row r="29" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="70"/>
+      <c r="A29" s="77"/>
       <c r="B29" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
       <c r="L29" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="M29" s="78"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="6"/>
+      <c r="M29" s="66"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="84"/>
       <c r="R29" s="6"/>
     </row>
     <row r="30" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="70"/>
+      <c r="A30" s="77"/>
       <c r="B30" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="59"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
       <c r="L30" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="M30" s="78"/>
-      <c r="N30" s="59"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="6"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="63"/>
+      <c r="P30" s="63"/>
+      <c r="Q30" s="84"/>
       <c r="R30" s="6"/>
     </row>
     <row r="31" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="70"/>
+      <c r="A31" s="77"/>
       <c r="B31" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
       <c r="L31" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="M31" s="78"/>
-      <c r="N31" s="59"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="6"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="84"/>
       <c r="R31" s="6"/>
     </row>
     <row r="32" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="70"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="59"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
       <c r="L32" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="M32" s="78"/>
-      <c r="N32" s="59"/>
-      <c r="O32" s="59"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="6"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="84"/>
       <c r="R32" s="6"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="70"/>
+      <c r="A33" s="77"/>
       <c r="B33" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="51" t="s">
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="M33" s="78"/>
-      <c r="N33" s="59"/>
-      <c r="O33" s="59"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="6"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="84"/>
       <c r="R33" s="6"/>
     </row>
     <row r="34" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="70"/>
+      <c r="A34" s="77"/>
       <c r="B34" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="59"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
       <c r="L34" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M34" s="78"/>
-      <c r="N34" s="59"/>
-      <c r="O34" s="59"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="6"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="63"/>
+      <c r="O34" s="63"/>
+      <c r="P34" s="63"/>
+      <c r="Q34" s="84"/>
       <c r="R34" s="6"/>
     </row>
     <row r="35" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="70"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="60"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
       <c r="L35" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="M35" s="80"/>
-      <c r="N35" s="60"/>
-      <c r="O35" s="60"/>
-      <c r="P35" s="60"/>
-      <c r="Q35" s="6"/>
+      <c r="M35" s="67"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="64"/>
+      <c r="Q35" s="85"/>
       <c r="R35" s="6"/>
     </row>
     <row r="36" spans="1:18" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="61" t="s">
+      <c r="A36" s="68" t="s">
         <v>272</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="C36" s="58" t="s">
+      <c r="C36" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="D36" s="58" t="s">
+      <c r="D36" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="F36" s="58" t="s">
+      <c r="F36" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="G36" s="58" t="s">
+      <c r="G36" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="H36" s="58" t="s">
+      <c r="H36" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="I36" s="58" t="s">
+      <c r="I36" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="J36" s="58" t="s">
+      <c r="J36" s="62" t="s">
         <v>259</v>
       </c>
-      <c r="K36" s="58" t="s">
+      <c r="K36" s="62" t="s">
         <v>260</v>
       </c>
       <c r="L36" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="M36" s="77" t="s">
+      <c r="M36" s="65" t="s">
         <v>285</v>
       </c>
-      <c r="N36" s="58" t="s">
+      <c r="N36" s="62" t="s">
         <v>293</v>
       </c>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="6"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="83" t="s">
+        <v>305</v>
+      </c>
       <c r="R36" s="6"/>
     </row>
     <row r="37" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="61"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
       <c r="L37" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="M37" s="78"/>
-      <c r="N37" s="59"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="6"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="63"/>
+      <c r="Q37" s="84"/>
       <c r="R37" s="6"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" s="61"/>
+      <c r="A38" s="68"/>
       <c r="B38" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="59"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
+      <c r="K38" s="63"/>
       <c r="L38" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="M38" s="78"/>
-      <c r="N38" s="59"/>
-      <c r="O38" s="59"/>
-      <c r="P38" s="59"/>
-      <c r="Q38" s="6"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="63"/>
+      <c r="O38" s="63"/>
+      <c r="P38" s="63"/>
+      <c r="Q38" s="84"/>
       <c r="R38" s="6"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="61"/>
+      <c r="A39" s="68"/>
       <c r="B39" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
       <c r="L39" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="M39" s="78"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="6"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="63"/>
+      <c r="P39" s="63"/>
+      <c r="Q39" s="84"/>
       <c r="R39" s="6"/>
     </row>
     <row r="40" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="61"/>
+      <c r="A40" s="68"/>
       <c r="B40" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="59"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="63"/>
+      <c r="K40" s="63"/>
       <c r="L40" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="M40" s="78"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="6"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="63"/>
+      <c r="O40" s="63"/>
+      <c r="P40" s="63"/>
+      <c r="Q40" s="84"/>
       <c r="R40" s="6"/>
     </row>
     <row r="41" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="61"/>
+      <c r="A41" s="68"/>
       <c r="B41" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="59"/>
-      <c r="K41" s="59"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
       <c r="L41" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="M41" s="78"/>
-      <c r="N41" s="59"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="59"/>
-      <c r="Q41" s="6"/>
+      <c r="M41" s="66"/>
+      <c r="N41" s="63"/>
+      <c r="O41" s="63"/>
+      <c r="P41" s="63"/>
+      <c r="Q41" s="84"/>
       <c r="R41" s="6"/>
     </row>
     <row r="42" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="61"/>
+      <c r="A42" s="68"/>
       <c r="B42" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
       <c r="L42" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="M42" s="78"/>
-      <c r="N42" s="59"/>
-      <c r="O42" s="59"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="6"/>
+      <c r="M42" s="66"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="84"/>
       <c r="R42" s="6"/>
     </row>
     <row r="43" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="61"/>
+      <c r="A43" s="68"/>
       <c r="B43" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="C43" s="59"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="59"/>
-      <c r="K43" s="59"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
       <c r="L43" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="M43" s="78"/>
-      <c r="N43" s="59"/>
-      <c r="O43" s="59"/>
-      <c r="P43" s="59"/>
-      <c r="Q43" s="42"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="84"/>
       <c r="R43" s="6"/>
     </row>
     <row r="44" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="61"/>
+      <c r="A44" s="68"/>
       <c r="B44" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
-      <c r="K44" s="59"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
       <c r="L44" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="M44" s="78"/>
-      <c r="N44" s="59"/>
-      <c r="O44" s="59"/>
-      <c r="P44" s="59"/>
-      <c r="Q44" s="42"/>
-      <c r="R44" s="42"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="84"/>
+      <c r="R44" s="40"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="61"/>
+      <c r="A45" s="68"/>
       <c r="B45" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="59"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="63"/>
       <c r="L45" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="M45" s="78"/>
-      <c r="N45" s="59"/>
-      <c r="O45" s="59"/>
-      <c r="P45" s="59"/>
-      <c r="Q45" s="42"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="63"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="63"/>
+      <c r="Q45" s="84"/>
       <c r="R45" s="6"/>
     </row>
     <row r="46" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="61"/>
+      <c r="A46" s="68"/>
       <c r="B46" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
       <c r="L46" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="M46" s="78"/>
-      <c r="N46" s="59"/>
-      <c r="O46" s="59"/>
-      <c r="P46" s="59"/>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="42"/>
+      <c r="M46" s="66"/>
+      <c r="N46" s="63"/>
+      <c r="O46" s="63"/>
+      <c r="P46" s="63"/>
+      <c r="Q46" s="84"/>
+      <c r="R46" s="40"/>
     </row>
     <row r="47" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="61"/>
+      <c r="A47" s="68"/>
       <c r="B47" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
       <c r="L47" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="M47" s="78"/>
-      <c r="N47" s="59"/>
-      <c r="O47" s="59"/>
-      <c r="P47" s="59"/>
-      <c r="Q47" s="42"/>
-      <c r="R47" s="42"/>
+      <c r="M47" s="66"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="63"/>
+      <c r="P47" s="63"/>
+      <c r="Q47" s="84"/>
+      <c r="R47" s="40"/>
     </row>
     <row r="48" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="61"/>
+      <c r="A48" s="68"/>
       <c r="B48" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="63"/>
       <c r="L48" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="M48" s="78"/>
-      <c r="N48" s="59"/>
-      <c r="O48" s="59"/>
-      <c r="P48" s="59"/>
-      <c r="Q48" s="42"/>
-      <c r="R48" s="42"/>
+      <c r="M48" s="66"/>
+      <c r="N48" s="63"/>
+      <c r="O48" s="63"/>
+      <c r="P48" s="63"/>
+      <c r="Q48" s="84"/>
+      <c r="R48" s="40"/>
     </row>
     <row r="49" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="61"/>
+      <c r="A49" s="68"/>
       <c r="B49" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="60"/>
-      <c r="H49" s="60"/>
-      <c r="I49" s="60"/>
-      <c r="J49" s="60"/>
-      <c r="K49" s="60"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="64"/>
+      <c r="K49" s="64"/>
       <c r="L49" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="M49" s="80"/>
-      <c r="N49" s="60"/>
-      <c r="O49" s="60"/>
-      <c r="P49" s="60"/>
-      <c r="Q49" s="42"/>
-      <c r="R49" s="42"/>
+      <c r="M49" s="67"/>
+      <c r="N49" s="64"/>
+      <c r="O49" s="64"/>
+      <c r="P49" s="64"/>
+      <c r="Q49" s="85"/>
+      <c r="R49" s="40"/>
     </row>
     <row r="50" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="62" t="s">
         <v>270</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="C50" s="71" t="s">
+      <c r="C50" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="D50" s="71" t="s">
+      <c r="D50" s="56" t="s">
         <v>286</v>
       </c>
-      <c r="E50" s="71" t="s">
+      <c r="E50" s="56" t="s">
         <v>255</v>
       </c>
-      <c r="F50" s="71" t="s">
+      <c r="F50" s="56" t="s">
         <v>253</v>
       </c>
-      <c r="G50" s="71" t="s">
+      <c r="G50" s="56" t="s">
         <v>254</v>
       </c>
-      <c r="H50" s="71" t="s">
+      <c r="H50" s="56" t="s">
         <v>252</v>
       </c>
-      <c r="I50" s="71" t="s">
+      <c r="I50" s="56" t="s">
         <v>256</v>
       </c>
-      <c r="J50" s="71" t="s">
+      <c r="J50" s="56" t="s">
         <v>259</v>
       </c>
-      <c r="K50" s="71" t="s">
+      <c r="K50" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="L50" s="49" t="s">
+      <c r="L50" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="M50" s="81" t="s">
+      <c r="M50" s="59" t="s">
         <v>285</v>
       </c>
-      <c r="N50" s="71" t="s">
+      <c r="N50" s="56" t="s">
         <v>294</v>
       </c>
-      <c r="O50" s="71"/>
-      <c r="P50" s="71"/>
-      <c r="Q50" s="42"/>
-      <c r="R50" s="42"/>
+      <c r="O50" s="56"/>
+      <c r="P50" s="56"/>
+      <c r="Q50" s="83" t="s">
+        <v>306</v>
+      </c>
+      <c r="R50" s="40"/>
     </row>
     <row r="51" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="59"/>
+      <c r="A51" s="63"/>
       <c r="B51" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="72"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
       <c r="L51" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="M51" s="82"/>
-      <c r="N51" s="72"/>
-      <c r="O51" s="72"/>
-      <c r="P51" s="72"/>
-      <c r="Q51" s="42"/>
-      <c r="R51" s="42"/>
+      <c r="M51" s="60"/>
+      <c r="N51" s="57"/>
+      <c r="O51" s="57"/>
+      <c r="P51" s="57"/>
+      <c r="Q51" s="84"/>
+      <c r="R51" s="40"/>
     </row>
     <row r="52" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="59"/>
+      <c r="A52" s="63"/>
       <c r="B52" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="72"/>
-      <c r="K52" s="72"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
       <c r="L52" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="M52" s="82"/>
-      <c r="N52" s="72"/>
-      <c r="O52" s="72"/>
-      <c r="P52" s="72"/>
-      <c r="Q52" s="42"/>
-      <c r="R52" s="42"/>
+      <c r="M52" s="60"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="84"/>
+      <c r="R52" s="40"/>
     </row>
     <row r="53" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="C53" s="73"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="73"/>
-      <c r="G53" s="73"/>
-      <c r="H53" s="73"/>
-      <c r="I53" s="73"/>
-      <c r="J53" s="73"/>
-      <c r="K53" s="73"/>
-      <c r="L53" s="50" t="s">
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="58"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="M53" s="83"/>
-      <c r="N53" s="73"/>
-      <c r="O53" s="73"/>
-      <c r="P53" s="73"/>
-      <c r="Q53" s="42"/>
-      <c r="R53" s="42"/>
+      <c r="M53" s="61"/>
+      <c r="N53" s="58"/>
+      <c r="O53" s="58"/>
+      <c r="P53" s="58"/>
+      <c r="Q53" s="85"/>
+      <c r="R53" s="40"/>
     </row>
     <row r="54" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="30" t="s">
@@ -4117,14 +4217,14 @@
       <c r="J54" s="36"/>
       <c r="K54" s="37"/>
       <c r="L54" s="37"/>
-      <c r="M54" s="55" t="s">
+      <c r="M54" s="53" t="s">
         <v>285</v>
       </c>
       <c r="N54" s="37"/>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
-      <c r="Q54" s="42"/>
-      <c r="R54" s="42"/>
+      <c r="Q54" s="86"/>
+      <c r="R54" s="40"/>
     </row>
     <row r="55" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="30" t="s">
@@ -4141,14 +4241,14 @@
       <c r="J55" s="36"/>
       <c r="K55" s="37"/>
       <c r="L55" s="37"/>
-      <c r="M55" s="55" t="s">
+      <c r="M55" s="53" t="s">
         <v>285</v>
       </c>
       <c r="N55" s="37"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
-      <c r="Q55" s="42"/>
-      <c r="R55" s="42"/>
+      <c r="Q55" s="87"/>
+      <c r="R55" s="40"/>
     </row>
     <row r="56" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30" t="s">
@@ -4163,15 +4263,15 @@
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="36"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
-      <c r="M56" s="56" t="s">
+      <c r="K56" s="41"/>
+      <c r="L56" s="41"/>
+      <c r="M56" s="54" t="s">
         <v>285</v>
       </c>
-      <c r="N56" s="43"/>
+      <c r="N56" s="41"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
-      <c r="Q56" s="42"/>
+      <c r="Q56" s="86"/>
       <c r="R56" s="6"/>
     </row>
     <row r="57" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4187,15 +4287,15 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="36"/>
-      <c r="K57" s="44"/>
-      <c r="L57" s="44"/>
-      <c r="M57" s="57" t="s">
+      <c r="K57" s="42"/>
+      <c r="L57" s="42"/>
+      <c r="M57" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="N57" s="44"/>
+      <c r="N57" s="42"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
-      <c r="Q57" s="42"/>
+      <c r="Q57" s="86"/>
       <c r="R57" s="6"/>
     </row>
     <row r="58" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4211,15 +4311,15 @@
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="36"/>
-      <c r="K58" s="44"/>
-      <c r="L58" s="44"/>
-      <c r="M58" s="57" t="s">
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="N58" s="44"/>
+      <c r="N58" s="42"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
-      <c r="Q58" s="42"/>
+      <c r="Q58" s="87"/>
       <c r="R58" s="6"/>
     </row>
     <row r="59" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4235,19 +4335,19 @@
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="36"/>
-      <c r="K59" s="44"/>
-      <c r="L59" s="44"/>
-      <c r="M59" s="57" t="s">
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
+      <c r="M59" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="N59" s="44"/>
+      <c r="N59" s="42"/>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
-      <c r="Q59" s="42"/>
+      <c r="Q59" s="87"/>
       <c r="R59" s="6"/>
     </row>
     <row r="60" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="52" t="s">
+      <c r="A60" s="50" t="s">
         <v>271</v>
       </c>
       <c r="B60" s="5"/>
@@ -4259,15 +4359,15 @@
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
-      <c r="K60" s="44"/>
-      <c r="L60" s="44"/>
-      <c r="M60" s="57" t="s">
+      <c r="K60" s="42"/>
+      <c r="L60" s="42"/>
+      <c r="M60" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="N60" s="44"/>
+      <c r="N60" s="42"/>
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
-      <c r="Q60" s="6"/>
+      <c r="Q60" s="86"/>
       <c r="R60" s="6"/>
     </row>
     <row r="61" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4283,15 +4383,15 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
-      <c r="K61" s="44"/>
-      <c r="L61" s="44"/>
-      <c r="M61" s="57" t="s">
+      <c r="K61" s="42"/>
+      <c r="L61" s="42"/>
+      <c r="M61" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="N61" s="44"/>
+      <c r="N61" s="42"/>
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
-      <c r="Q61" s="6"/>
+      <c r="Q61" s="88"/>
       <c r="R61" s="6"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
@@ -4305,10 +4405,10 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
-      <c r="K62" s="44"/>
-      <c r="L62" s="44"/>
-      <c r="M62" s="44"/>
-      <c r="N62" s="44"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="42"/>
+      <c r="M62" s="42"/>
+      <c r="N62" s="42"/>
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
       <c r="Q62" s="6"/>
@@ -4325,10 +4425,10 @@
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
-      <c r="K63" s="44"/>
-      <c r="L63" s="44"/>
-      <c r="M63" s="44"/>
-      <c r="N63" s="44"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="42"/>
+      <c r="M63" s="42"/>
+      <c r="N63" s="42"/>
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
       <c r="Q63" s="6"/>
@@ -4345,10 +4445,10 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
-      <c r="K64" s="44"/>
-      <c r="L64" s="44"/>
-      <c r="M64" s="44"/>
-      <c r="N64" s="44"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="42"/>
+      <c r="M64" s="42"/>
+      <c r="N64" s="42"/>
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
       <c r="Q64" s="6"/>
@@ -4365,10 +4465,10 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
-      <c r="K65" s="44"/>
-      <c r="L65" s="44"/>
-      <c r="M65" s="44"/>
-      <c r="N65" s="44"/>
+      <c r="K65" s="42"/>
+      <c r="L65" s="42"/>
+      <c r="M65" s="42"/>
+      <c r="N65" s="42"/>
       <c r="O65" s="5"/>
       <c r="P65" s="5"/>
       <c r="Q65" s="6"/>
@@ -4385,10 +4485,10 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
-      <c r="K66" s="44"/>
-      <c r="L66" s="44"/>
-      <c r="M66" s="44"/>
-      <c r="N66" s="44"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="42"/>
+      <c r="M66" s="42"/>
+      <c r="N66" s="42"/>
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
       <c r="Q66" s="6"/>
@@ -4405,10 +4505,10 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
-      <c r="K67" s="44"/>
-      <c r="L67" s="44"/>
-      <c r="M67" s="44"/>
-      <c r="N67" s="44"/>
+      <c r="K67" s="42"/>
+      <c r="L67" s="42"/>
+      <c r="M67" s="42"/>
+      <c r="N67" s="42"/>
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
       <c r="Q67" s="6"/>
@@ -4425,10 +4525,10 @@
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
-      <c r="K68" s="44"/>
-      <c r="L68" s="44"/>
-      <c r="M68" s="44"/>
-      <c r="N68" s="44"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="42"/>
+      <c r="M68" s="42"/>
+      <c r="N68" s="42"/>
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
       <c r="Q68" s="6"/>
@@ -4445,10 +4545,10 @@
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
-      <c r="K69" s="44"/>
-      <c r="L69" s="44"/>
-      <c r="M69" s="44"/>
-      <c r="N69" s="44"/>
+      <c r="K69" s="42"/>
+      <c r="L69" s="42"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="42"/>
       <c r="O69" s="5"/>
       <c r="P69" s="5"/>
       <c r="Q69" s="6"/>
@@ -4465,10 +4565,10 @@
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
-      <c r="K70" s="44"/>
-      <c r="L70" s="44"/>
-      <c r="M70" s="44"/>
-      <c r="N70" s="44"/>
+      <c r="K70" s="42"/>
+      <c r="L70" s="42"/>
+      <c r="M70" s="42"/>
+      <c r="N70" s="42"/>
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
       <c r="Q70" s="6"/>
@@ -4485,14 +4585,14 @@
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
-      <c r="K71" s="44"/>
-      <c r="L71" s="44"/>
-      <c r="M71" s="44"/>
-      <c r="N71" s="44"/>
+      <c r="K71" s="42"/>
+      <c r="L71" s="42"/>
+      <c r="M71" s="42"/>
+      <c r="N71" s="42"/>
       <c r="O71" s="5"/>
       <c r="P71" s="5"/>
       <c r="Q71" s="6"/>
-      <c r="R71" s="42"/>
+      <c r="R71" s="40"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
@@ -4505,14 +4605,14 @@
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
-      <c r="K72" s="44"/>
-      <c r="L72" s="44"/>
-      <c r="M72" s="44"/>
-      <c r="N72" s="44"/>
+      <c r="K72" s="42"/>
+      <c r="L72" s="42"/>
+      <c r="M72" s="42"/>
+      <c r="N72" s="42"/>
       <c r="O72" s="5"/>
       <c r="P72" s="5"/>
       <c r="Q72" s="6"/>
-      <c r="R72" s="42"/>
+      <c r="R72" s="40"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
@@ -4525,10 +4625,10 @@
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
-      <c r="K73" s="44"/>
-      <c r="L73" s="44"/>
-      <c r="M73" s="44"/>
-      <c r="N73" s="44"/>
+      <c r="K73" s="42"/>
+      <c r="L73" s="42"/>
+      <c r="M73" s="42"/>
+      <c r="N73" s="42"/>
       <c r="O73" s="5"/>
       <c r="P73" s="5"/>
       <c r="Q73" s="6"/>
@@ -4545,14 +4645,14 @@
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
-      <c r="K74" s="44"/>
-      <c r="L74" s="44"/>
-      <c r="M74" s="44"/>
-      <c r="N74" s="44"/>
+      <c r="K74" s="42"/>
+      <c r="L74" s="42"/>
+      <c r="M74" s="42"/>
+      <c r="N74" s="42"/>
       <c r="O74" s="5"/>
       <c r="P74" s="5"/>
       <c r="Q74" s="6"/>
-      <c r="R74" s="42"/>
+      <c r="R74" s="40"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
@@ -4565,10 +4665,10 @@
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
-      <c r="K75" s="44"/>
-      <c r="L75" s="44"/>
-      <c r="M75" s="44"/>
-      <c r="N75" s="44"/>
+      <c r="K75" s="42"/>
+      <c r="L75" s="42"/>
+      <c r="M75" s="42"/>
+      <c r="N75" s="42"/>
       <c r="O75" s="5"/>
       <c r="P75" s="5"/>
       <c r="Q75" s="6"/>
@@ -4585,10 +4685,10 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
-      <c r="K76" s="44"/>
-      <c r="L76" s="44"/>
-      <c r="M76" s="44"/>
-      <c r="N76" s="44"/>
+      <c r="K76" s="42"/>
+      <c r="L76" s="42"/>
+      <c r="M76" s="42"/>
+      <c r="N76" s="42"/>
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
       <c r="Q76" s="6"/>
@@ -4605,10 +4705,10 @@
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
-      <c r="K77" s="44"/>
-      <c r="L77" s="44"/>
-      <c r="M77" s="44"/>
-      <c r="N77" s="44"/>
+      <c r="K77" s="42"/>
+      <c r="L77" s="42"/>
+      <c r="M77" s="42"/>
+      <c r="N77" s="42"/>
       <c r="O77" s="5"/>
       <c r="P77" s="5"/>
       <c r="Q77" s="6"/>
@@ -4625,10 +4725,10 @@
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
-      <c r="K78" s="44"/>
-      <c r="L78" s="44"/>
-      <c r="M78" s="44"/>
-      <c r="N78" s="44"/>
+      <c r="K78" s="42"/>
+      <c r="L78" s="42"/>
+      <c r="M78" s="42"/>
+      <c r="N78" s="42"/>
       <c r="O78" s="5"/>
       <c r="P78" s="5"/>
       <c r="Q78" s="6"/>
@@ -4665,10 +4765,10 @@
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
-      <c r="K80" s="44"/>
-      <c r="L80" s="44"/>
-      <c r="M80" s="44"/>
-      <c r="N80" s="44"/>
+      <c r="K80" s="42"/>
+      <c r="L80" s="42"/>
+      <c r="M80" s="42"/>
+      <c r="N80" s="42"/>
       <c r="O80" s="5"/>
       <c r="P80" s="5"/>
       <c r="Q80" s="6"/>
@@ -4685,10 +4785,10 @@
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
-      <c r="K81" s="44"/>
-      <c r="L81" s="44"/>
-      <c r="M81" s="44"/>
-      <c r="N81" s="44"/>
+      <c r="K81" s="42"/>
+      <c r="L81" s="42"/>
+      <c r="M81" s="42"/>
+      <c r="N81" s="42"/>
       <c r="O81" s="5"/>
       <c r="P81" s="5"/>
       <c r="Q81" s="6"/>
@@ -4705,10 +4805,10 @@
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
-      <c r="K82" s="44"/>
-      <c r="L82" s="44"/>
-      <c r="M82" s="44"/>
-      <c r="N82" s="44"/>
+      <c r="K82" s="42"/>
+      <c r="L82" s="42"/>
+      <c r="M82" s="42"/>
+      <c r="N82" s="42"/>
       <c r="O82" s="5"/>
       <c r="P82" s="5"/>
       <c r="Q82" s="6"/>
@@ -4725,10 +4825,10 @@
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
-      <c r="K83" s="44"/>
-      <c r="L83" s="44"/>
-      <c r="M83" s="44"/>
-      <c r="N83" s="44"/>
+      <c r="K83" s="42"/>
+      <c r="L83" s="42"/>
+      <c r="M83" s="42"/>
+      <c r="N83" s="42"/>
       <c r="O83" s="5"/>
       <c r="P83" s="5"/>
       <c r="Q83" s="6"/>
@@ -4745,10 +4845,10 @@
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
-      <c r="K84" s="44"/>
-      <c r="L84" s="44"/>
-      <c r="M84" s="44"/>
-      <c r="N84" s="44"/>
+      <c r="K84" s="42"/>
+      <c r="L84" s="42"/>
+      <c r="M84" s="42"/>
+      <c r="N84" s="42"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
       <c r="Q84" s="6"/>
@@ -4765,14 +4865,14 @@
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="5"/>
-      <c r="K85" s="44"/>
-      <c r="L85" s="44"/>
-      <c r="M85" s="44"/>
-      <c r="N85" s="44"/>
+      <c r="K85" s="42"/>
+      <c r="L85" s="42"/>
+      <c r="M85" s="42"/>
+      <c r="N85" s="42"/>
       <c r="O85" s="5"/>
       <c r="P85" s="5"/>
       <c r="Q85" s="6"/>
-      <c r="R85" s="42"/>
+      <c r="R85" s="40"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
@@ -4785,10 +4885,10 @@
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
-      <c r="K86" s="44"/>
-      <c r="L86" s="44"/>
-      <c r="M86" s="44"/>
-      <c r="N86" s="44"/>
+      <c r="K86" s="42"/>
+      <c r="L86" s="42"/>
+      <c r="M86" s="42"/>
+      <c r="N86" s="42"/>
       <c r="O86" s="5"/>
       <c r="P86" s="5"/>
       <c r="Q86" s="6"/>
@@ -4805,10 +4905,10 @@
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="5"/>
-      <c r="K87" s="44"/>
-      <c r="L87" s="44"/>
-      <c r="M87" s="44"/>
-      <c r="N87" s="44"/>
+      <c r="K87" s="42"/>
+      <c r="L87" s="42"/>
+      <c r="M87" s="42"/>
+      <c r="N87" s="42"/>
       <c r="O87" s="5"/>
       <c r="P87" s="5"/>
       <c r="Q87" s="6"/>
@@ -4825,10 +4925,10 @@
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
-      <c r="K88" s="44"/>
-      <c r="L88" s="44"/>
-      <c r="M88" s="44"/>
-      <c r="N88" s="44"/>
+      <c r="K88" s="42"/>
+      <c r="L88" s="42"/>
+      <c r="M88" s="42"/>
+      <c r="N88" s="42"/>
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
       <c r="Q88" s="6"/>
@@ -4845,10 +4945,10 @@
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
-      <c r="K89" s="44"/>
-      <c r="L89" s="44"/>
-      <c r="M89" s="44"/>
-      <c r="N89" s="44"/>
+      <c r="K89" s="42"/>
+      <c r="L89" s="42"/>
+      <c r="M89" s="42"/>
+      <c r="N89" s="42"/>
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
       <c r="Q89" s="6"/>
@@ -4865,10 +4965,10 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
-      <c r="K90" s="44"/>
-      <c r="L90" s="44"/>
-      <c r="M90" s="44"/>
-      <c r="N90" s="44"/>
+      <c r="K90" s="42"/>
+      <c r="L90" s="42"/>
+      <c r="M90" s="42"/>
+      <c r="N90" s="42"/>
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
       <c r="Q90" s="6"/>
@@ -6584,7 +6684,7 @@
       <c r="G176" s="5"/>
       <c r="H176" s="5"/>
       <c r="I176" s="5"/>
-      <c r="J176" s="45"/>
+      <c r="J176" s="43"/>
       <c r="K176" s="36"/>
       <c r="L176" s="36"/>
       <c r="M176" s="36"/>
@@ -6624,7 +6724,7 @@
       <c r="G178" s="5"/>
       <c r="H178" s="5"/>
       <c r="I178" s="5"/>
-      <c r="J178" s="45"/>
+      <c r="J178" s="43"/>
       <c r="K178" s="36"/>
       <c r="L178" s="36"/>
       <c r="M178" s="36"/>
@@ -6644,7 +6744,7 @@
       <c r="G179" s="5"/>
       <c r="H179" s="5"/>
       <c r="I179" s="5"/>
-      <c r="J179" s="45"/>
+      <c r="J179" s="43"/>
       <c r="K179" s="36"/>
       <c r="L179" s="36"/>
       <c r="M179" s="36"/>
@@ -6664,7 +6764,7 @@
       <c r="G180" s="5"/>
       <c r="H180" s="5"/>
       <c r="I180" s="5"/>
-      <c r="J180" s="45"/>
+      <c r="J180" s="43"/>
       <c r="K180" s="36"/>
       <c r="L180" s="36"/>
       <c r="M180" s="36"/>
@@ -6684,7 +6784,7 @@
       <c r="G181" s="5"/>
       <c r="H181" s="5"/>
       <c r="I181" s="5"/>
-      <c r="J181" s="45"/>
+      <c r="J181" s="43"/>
       <c r="K181" s="36"/>
       <c r="L181" s="36"/>
       <c r="M181" s="36"/>
@@ -6704,7 +6804,7 @@
       <c r="G182" s="5"/>
       <c r="H182" s="5"/>
       <c r="I182" s="5"/>
-      <c r="J182" s="45"/>
+      <c r="J182" s="43"/>
       <c r="K182" s="36"/>
       <c r="L182" s="36"/>
       <c r="M182" s="36"/>
@@ -6735,15 +6835,74 @@
       <c r="R183" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="H50:H53"/>
-    <mergeCell ref="I50:I53"/>
-    <mergeCell ref="P50:P53"/>
-    <mergeCell ref="O50:O53"/>
-    <mergeCell ref="J50:J53"/>
-    <mergeCell ref="K50:K53"/>
-    <mergeCell ref="M50:M53"/>
-    <mergeCell ref="N50:N53"/>
+  <mergeCells count="91">
+    <mergeCell ref="Q50:Q53"/>
+    <mergeCell ref="Q36:Q49"/>
+    <mergeCell ref="Q4:Q12"/>
+    <mergeCell ref="Q13:Q20"/>
+    <mergeCell ref="Q21:Q25"/>
+    <mergeCell ref="Q28:Q35"/>
+    <mergeCell ref="C36:C49"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="H4:H12"/>
+    <mergeCell ref="H13:H20"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="I13:I20"/>
+    <mergeCell ref="J13:J20"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="I4:I12"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="D4:D12"/>
+    <mergeCell ref="F4:F12"/>
+    <mergeCell ref="G4:G12"/>
+    <mergeCell ref="D13:D20"/>
+    <mergeCell ref="E13:E20"/>
+    <mergeCell ref="F13:F20"/>
+    <mergeCell ref="G13:G20"/>
+    <mergeCell ref="D28:D35"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C28:C35"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="C13:C20"/>
+    <mergeCell ref="J28:J35"/>
+    <mergeCell ref="K28:K35"/>
+    <mergeCell ref="H28:H35"/>
+    <mergeCell ref="H36:H49"/>
+    <mergeCell ref="E4:E12"/>
+    <mergeCell ref="E28:E35"/>
+    <mergeCell ref="F28:F35"/>
+    <mergeCell ref="G28:G35"/>
+    <mergeCell ref="I28:I35"/>
+    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="G21:G25"/>
+    <mergeCell ref="J4:J12"/>
+    <mergeCell ref="M4:M12"/>
+    <mergeCell ref="N4:N12"/>
+    <mergeCell ref="O4:O12"/>
+    <mergeCell ref="P4:P12"/>
+    <mergeCell ref="K13:K20"/>
+    <mergeCell ref="M13:M20"/>
+    <mergeCell ref="N13:N20"/>
+    <mergeCell ref="O13:O20"/>
+    <mergeCell ref="P13:P20"/>
+    <mergeCell ref="K4:K12"/>
+    <mergeCell ref="O36:O49"/>
+    <mergeCell ref="P36:P49"/>
+    <mergeCell ref="M21:M25"/>
+    <mergeCell ref="N21:N25"/>
+    <mergeCell ref="O21:O25"/>
+    <mergeCell ref="P21:P25"/>
+    <mergeCell ref="M28:M35"/>
+    <mergeCell ref="N28:N35"/>
+    <mergeCell ref="O28:O35"/>
+    <mergeCell ref="P28:P35"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="C50:C53"/>
     <mergeCell ref="D50:D53"/>
@@ -6760,67 +6919,14 @@
     <mergeCell ref="E50:E53"/>
     <mergeCell ref="F50:F53"/>
     <mergeCell ref="G50:G53"/>
-    <mergeCell ref="O36:O49"/>
-    <mergeCell ref="P36:P49"/>
-    <mergeCell ref="M21:M25"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="M28:M35"/>
-    <mergeCell ref="N28:N35"/>
-    <mergeCell ref="O28:O35"/>
-    <mergeCell ref="P28:P35"/>
-    <mergeCell ref="M4:M12"/>
-    <mergeCell ref="N4:N12"/>
-    <mergeCell ref="O4:O12"/>
-    <mergeCell ref="P4:P12"/>
-    <mergeCell ref="K13:K20"/>
-    <mergeCell ref="M13:M20"/>
-    <mergeCell ref="N13:N20"/>
-    <mergeCell ref="O13:O20"/>
-    <mergeCell ref="P13:P20"/>
-    <mergeCell ref="K4:K12"/>
-    <mergeCell ref="J28:J35"/>
-    <mergeCell ref="K28:K35"/>
-    <mergeCell ref="H28:H35"/>
-    <mergeCell ref="H36:H49"/>
-    <mergeCell ref="E4:E12"/>
-    <mergeCell ref="E28:E35"/>
-    <mergeCell ref="F28:F35"/>
-    <mergeCell ref="G28:G35"/>
-    <mergeCell ref="I28:I35"/>
-    <mergeCell ref="F21:F25"/>
-    <mergeCell ref="G21:G25"/>
-    <mergeCell ref="J4:J12"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="D4:D12"/>
-    <mergeCell ref="F4:F12"/>
-    <mergeCell ref="G4:G12"/>
-    <mergeCell ref="D13:D20"/>
-    <mergeCell ref="E13:E20"/>
-    <mergeCell ref="F13:F20"/>
-    <mergeCell ref="G13:G20"/>
-    <mergeCell ref="D28:D35"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C28:C35"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="C13:C20"/>
-    <mergeCell ref="C36:C49"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="H4:H12"/>
-    <mergeCell ref="H13:H20"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="I13:I20"/>
-    <mergeCell ref="J13:J20"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="I4:I12"/>
+    <mergeCell ref="H50:H53"/>
+    <mergeCell ref="I50:I53"/>
+    <mergeCell ref="P50:P53"/>
+    <mergeCell ref="O50:O53"/>
+    <mergeCell ref="J50:J53"/>
+    <mergeCell ref="K50:K53"/>
+    <mergeCell ref="M50:M53"/>
+    <mergeCell ref="N50:N53"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1"/>
@@ -6871,15 +6977,24 @@
     <hyperlink ref="L52" r:id="rId46"/>
     <hyperlink ref="L51" r:id="rId47"/>
     <hyperlink ref="L53" r:id="rId48"/>
+    <hyperlink ref="Q3" r:id="rId49"/>
+    <hyperlink ref="Q4" r:id="rId50"/>
+    <hyperlink ref="Q13" r:id="rId51"/>
+    <hyperlink ref="Q21" r:id="rId52"/>
+    <hyperlink ref="Q26" r:id="rId53"/>
+    <hyperlink ref="Q27" r:id="rId54"/>
+    <hyperlink ref="Q28" r:id="rId55"/>
+    <hyperlink ref="Q36" r:id="rId56"/>
+    <hyperlink ref="Q50" r:id="rId57"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId49"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId58"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Predeterminado"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Predeterminado"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId50"/>
-  <legacyDrawing r:id="rId51"/>
+  <drawing r:id="rId59"/>
+  <legacyDrawing r:id="rId60"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Subcategorias de Vida Estudiantil
Ficha para subida de recurso Educatico
</commit_message>
<xml_diff>
--- a/documentacion/vidaestudiantil/Subida a Educatico/ficha_educatico-AGENDAESTUDIANTL.xlsx
+++ b/documentacion/vidaestudiantil/Subida a Educatico/ficha_educatico-AGENDAESTUDIANTL.xlsx
@@ -1612,7 +1612,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1658,6 +1658,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1784,7 +1790,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1951,6 +1957,87 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1969,85 +2056,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2660,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2681,24 +2690,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="67" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
       <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="1:18" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2750,7 +2759,7 @@
       <c r="P2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="82" t="s">
+      <c r="Q2" s="56" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2799,613 +2808,613 @@
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="86" t="s">
+      <c r="Q3" s="89" t="s">
         <v>299</v>
       </c>
       <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="70" t="s">
         <v>278</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="63" t="s">
         <v>251</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="63" t="s">
         <v>286</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="63" t="s">
         <v>253</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="63" t="s">
         <v>254</v>
       </c>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="71" t="s">
         <v>252</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="71" t="s">
         <v>256</v>
       </c>
-      <c r="J4" s="73" t="s">
+      <c r="J4" s="71" t="s">
         <v>259</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="71" t="s">
         <v>260</v>
       </c>
       <c r="L4" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="70" t="s">
+      <c r="M4" s="76" t="s">
         <v>285</v>
       </c>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="83" t="s">
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="60" t="s">
         <v>299</v>
       </c>
       <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="81"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="M5" s="71"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="84"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="61"/>
       <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="81"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
       <c r="L6" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="M6" s="71"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="84"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="61"/>
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="81"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
       <c r="L7" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="M7" s="71"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="84"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="61"/>
       <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="81"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
       <c r="L8" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="M8" s="71"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="84"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="61"/>
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="81"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
       <c r="L9" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="M9" s="71"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="84"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="61"/>
       <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="81"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
       <c r="L10" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="M10" s="71"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="84"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="61"/>
       <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="81"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
       <c r="L11" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="M11" s="71"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="84"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="61"/>
       <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="81"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
       <c r="L12" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="M12" s="72"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="85"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="62"/>
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="70" t="s">
         <v>276</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="63" t="s">
         <v>251</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="63" t="s">
         <v>286</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="63" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="63" t="s">
         <v>253</v>
       </c>
-      <c r="G13" s="62" t="s">
+      <c r="G13" s="63" t="s">
         <v>254</v>
       </c>
-      <c r="H13" s="62" t="s">
+      <c r="H13" s="63" t="s">
         <v>252</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="63" t="s">
         <v>256</v>
       </c>
-      <c r="J13" s="62" t="s">
+      <c r="J13" s="63" t="s">
         <v>259</v>
       </c>
-      <c r="K13" s="62" t="s">
+      <c r="K13" s="63" t="s">
         <v>260</v>
       </c>
       <c r="L13" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="M13" s="65" t="s">
+      <c r="M13" s="79" t="s">
         <v>285</v>
       </c>
-      <c r="N13" s="62" t="s">
+      <c r="N13" s="63" t="s">
         <v>289</v>
       </c>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="83" t="s">
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="60" t="s">
         <v>300</v>
       </c>
       <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="81"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
       <c r="L14" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="M14" s="66"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="84"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="64"/>
+      <c r="Q14" s="61"/>
       <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="81"/>
+      <c r="A15" s="70"/>
       <c r="B15" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
       <c r="L15" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="M15" s="66"/>
-      <c r="N15" s="63"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="84"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="64"/>
+      <c r="Q15" s="61"/>
       <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="81"/>
+      <c r="A16" s="70"/>
       <c r="B16" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
       <c r="L16" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="M16" s="66"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="84"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="61"/>
       <c r="R16" s="6"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="81"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
       <c r="L17" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="M17" s="66"/>
-      <c r="N17" s="63"/>
-      <c r="O17" s="63"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="84"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="64"/>
+      <c r="Q17" s="61"/>
       <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="81"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
       <c r="L18" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="M18" s="66"/>
-      <c r="N18" s="63"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="84"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="64"/>
+      <c r="P18" s="64"/>
+      <c r="Q18" s="61"/>
       <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="81"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="63"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
       <c r="L19" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="M19" s="66"/>
-      <c r="N19" s="63"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="63"/>
-      <c r="Q19" s="84"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="64"/>
+      <c r="Q19" s="61"/>
       <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="81"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
       <c r="L20" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="M20" s="66"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="85"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="64"/>
+      <c r="Q20" s="62"/>
       <c r="R20" s="6"/>
     </row>
     <row r="21" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="70" t="s">
         <v>275</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="68" t="s">
+      <c r="C21" s="66" t="s">
         <v>251</v>
       </c>
-      <c r="D21" s="68" t="s">
+      <c r="D21" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="66" t="s">
         <v>255</v>
       </c>
-      <c r="F21" s="68" t="s">
+      <c r="F21" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="H21" s="68" t="s">
+      <c r="H21" s="66" t="s">
         <v>252</v>
       </c>
-      <c r="I21" s="68" t="s">
+      <c r="I21" s="66" t="s">
         <v>256</v>
       </c>
-      <c r="J21" s="68" t="s">
+      <c r="J21" s="66" t="s">
         <v>259</v>
       </c>
-      <c r="K21" s="68" t="s">
+      <c r="K21" s="66" t="s">
         <v>260</v>
       </c>
       <c r="L21" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="M21" s="69"/>
-      <c r="N21" s="68" t="s">
+      <c r="M21" s="81"/>
+      <c r="N21" s="66" t="s">
         <v>290</v>
       </c>
-      <c r="O21" s="68"/>
-      <c r="P21" s="68"/>
-      <c r="Q21" s="83" t="s">
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="60" t="s">
         <v>301</v>
       </c>
       <c r="R21" s="6"/>
     </row>
     <row r="22" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="81"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
       <c r="L22" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="M22" s="69"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="84"/>
+      <c r="M22" s="81"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="61"/>
       <c r="R22" s="6"/>
     </row>
     <row r="23" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="81"/>
+      <c r="A23" s="70"/>
       <c r="B23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
       <c r="L23" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="M23" s="69"/>
-      <c r="N23" s="68"/>
-      <c r="O23" s="68"/>
-      <c r="P23" s="68"/>
-      <c r="Q23" s="84"/>
+      <c r="M23" s="81"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="61"/>
       <c r="R23" s="6"/>
     </row>
     <row r="24" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="81"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
       <c r="L24" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="M24" s="69"/>
-      <c r="N24" s="68"/>
-      <c r="O24" s="68"/>
-      <c r="P24" s="68"/>
-      <c r="Q24" s="84"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="66"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="61"/>
       <c r="R24" s="6"/>
     </row>
     <row r="25" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="81"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="66"/>
       <c r="L25" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="M25" s="69"/>
-      <c r="N25" s="68"/>
-      <c r="O25" s="68"/>
-      <c r="P25" s="68"/>
-      <c r="Q25" s="85"/>
+      <c r="M25" s="81"/>
+      <c r="N25" s="66"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="62"/>
       <c r="R25" s="6"/>
     </row>
     <row r="26" spans="1:18" ht="244.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3453,7 +3462,7 @@
       </c>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-      <c r="Q26" s="86" t="s">
+      <c r="Q26" s="57" t="s">
         <v>302</v>
       </c>
       <c r="R26" s="6"/>
@@ -3503,703 +3512,703 @@
       </c>
       <c r="O27" s="34"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="86" t="s">
+      <c r="Q27" s="57" t="s">
         <v>303</v>
       </c>
       <c r="R27" s="6"/>
     </row>
     <row r="28" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="74" t="s">
         <v>274</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="63" t="s">
         <v>251</v>
       </c>
-      <c r="D28" s="62" t="s">
+      <c r="D28" s="63" t="s">
         <v>286</v>
       </c>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62" t="s">
+      <c r="E28" s="63"/>
+      <c r="F28" s="63" t="s">
         <v>253</v>
       </c>
-      <c r="G28" s="62" t="s">
+      <c r="G28" s="63" t="s">
         <v>254</v>
       </c>
-      <c r="H28" s="62" t="s">
+      <c r="H28" s="63" t="s">
         <v>252</v>
       </c>
-      <c r="I28" s="62" t="s">
+      <c r="I28" s="63" t="s">
         <v>256</v>
       </c>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="M28" s="65"/>
-      <c r="N28" s="62" t="s">
+      <c r="M28" s="79"/>
+      <c r="N28" s="63" t="s">
         <v>295</v>
       </c>
-      <c r="O28" s="62"/>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="83" t="s">
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="60" t="s">
         <v>304</v>
       </c>
       <c r="R28" s="6"/>
     </row>
     <row r="29" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="77"/>
+      <c r="A29" s="75"/>
       <c r="B29" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="63"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
       <c r="L29" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="M29" s="66"/>
-      <c r="N29" s="63"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="84"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
+      <c r="Q29" s="61"/>
       <c r="R29" s="6"/>
     </row>
     <row r="30" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="77"/>
+      <c r="A30" s="75"/>
       <c r="B30" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="63"/>
-      <c r="K30" s="63"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
       <c r="L30" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="M30" s="66"/>
-      <c r="N30" s="63"/>
-      <c r="O30" s="63"/>
-      <c r="P30" s="63"/>
-      <c r="Q30" s="84"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="64"/>
+      <c r="Q30" s="61"/>
       <c r="R30" s="6"/>
     </row>
     <row r="31" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="77"/>
+      <c r="A31" s="75"/>
       <c r="B31" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
       <c r="L31" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="M31" s="66"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="84"/>
+      <c r="M31" s="80"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="64"/>
+      <c r="Q31" s="61"/>
       <c r="R31" s="6"/>
     </row>
     <row r="32" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="77"/>
+      <c r="A32" s="75"/>
       <c r="B32" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
       <c r="L32" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="M32" s="66"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="84"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="64"/>
+      <c r="Q32" s="61"/>
       <c r="R32" s="6"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="77"/>
+      <c r="A33" s="75"/>
       <c r="B33" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="63"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
       <c r="L33" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="M33" s="66"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="84"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="64"/>
+      <c r="Q33" s="61"/>
       <c r="R33" s="6"/>
     </row>
     <row r="34" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="77"/>
+      <c r="A34" s="75"/>
       <c r="B34" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
-      <c r="K34" s="63"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
       <c r="L34" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="M34" s="66"/>
-      <c r="N34" s="63"/>
-      <c r="O34" s="63"/>
-      <c r="P34" s="63"/>
-      <c r="Q34" s="84"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="64"/>
+      <c r="O34" s="64"/>
+      <c r="P34" s="64"/>
+      <c r="Q34" s="61"/>
       <c r="R34" s="6"/>
     </row>
     <row r="35" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="77"/>
+      <c r="A35" s="75"/>
       <c r="B35" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="64"/>
-      <c r="K35" s="64"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="65"/>
       <c r="L35" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="M35" s="67"/>
-      <c r="N35" s="64"/>
-      <c r="O35" s="64"/>
-      <c r="P35" s="64"/>
-      <c r="Q35" s="85"/>
+      <c r="M35" s="82"/>
+      <c r="N35" s="65"/>
+      <c r="O35" s="65"/>
+      <c r="P35" s="65"/>
+      <c r="Q35" s="62"/>
       <c r="R35" s="6"/>
     </row>
     <row r="36" spans="1:18" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="66" t="s">
         <v>272</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="C36" s="62" t="s">
+      <c r="C36" s="63" t="s">
         <v>251</v>
       </c>
-      <c r="D36" s="62" t="s">
+      <c r="D36" s="63" t="s">
         <v>286</v>
       </c>
-      <c r="E36" s="62" t="s">
+      <c r="E36" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="F36" s="62" t="s">
+      <c r="F36" s="63" t="s">
         <v>253</v>
       </c>
-      <c r="G36" s="62" t="s">
+      <c r="G36" s="63" t="s">
         <v>254</v>
       </c>
-      <c r="H36" s="62" t="s">
+      <c r="H36" s="63" t="s">
         <v>252</v>
       </c>
-      <c r="I36" s="62" t="s">
+      <c r="I36" s="63" t="s">
         <v>256</v>
       </c>
-      <c r="J36" s="62" t="s">
+      <c r="J36" s="63" t="s">
         <v>259</v>
       </c>
-      <c r="K36" s="62" t="s">
+      <c r="K36" s="63" t="s">
         <v>260</v>
       </c>
       <c r="L36" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="M36" s="65" t="s">
+      <c r="M36" s="79" t="s">
         <v>285</v>
       </c>
-      <c r="N36" s="62" t="s">
+      <c r="N36" s="63" t="s">
         <v>293</v>
       </c>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
-      <c r="Q36" s="83" t="s">
+      <c r="O36" s="63"/>
+      <c r="P36" s="63"/>
+      <c r="Q36" s="60" t="s">
         <v>305</v>
       </c>
       <c r="R36" s="6"/>
     </row>
     <row r="37" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="68"/>
+      <c r="A37" s="66"/>
       <c r="B37" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
-      <c r="K37" s="63"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+      <c r="K37" s="64"/>
       <c r="L37" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="M37" s="66"/>
-      <c r="N37" s="63"/>
-      <c r="O37" s="63"/>
-      <c r="P37" s="63"/>
-      <c r="Q37" s="84"/>
+      <c r="M37" s="80"/>
+      <c r="N37" s="64"/>
+      <c r="O37" s="64"/>
+      <c r="P37" s="64"/>
+      <c r="Q37" s="61"/>
       <c r="R37" s="6"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" s="68"/>
+      <c r="A38" s="66"/>
       <c r="B38" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
-      <c r="K38" s="63"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
       <c r="L38" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="M38" s="66"/>
-      <c r="N38" s="63"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="63"/>
-      <c r="Q38" s="84"/>
+      <c r="M38" s="80"/>
+      <c r="N38" s="64"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="64"/>
+      <c r="Q38" s="61"/>
       <c r="R38" s="6"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="68"/>
+      <c r="A39" s="66"/>
       <c r="B39" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="63"/>
-      <c r="K39" s="63"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
       <c r="L39" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="M39" s="66"/>
-      <c r="N39" s="63"/>
-      <c r="O39" s="63"/>
-      <c r="P39" s="63"/>
-      <c r="Q39" s="84"/>
+      <c r="M39" s="80"/>
+      <c r="N39" s="64"/>
+      <c r="O39" s="64"/>
+      <c r="P39" s="64"/>
+      <c r="Q39" s="61"/>
       <c r="R39" s="6"/>
     </row>
     <row r="40" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="68"/>
+      <c r="A40" s="66"/>
       <c r="B40" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="63"/>
-      <c r="K40" s="63"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="64"/>
       <c r="L40" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="M40" s="66"/>
-      <c r="N40" s="63"/>
-      <c r="O40" s="63"/>
-      <c r="P40" s="63"/>
-      <c r="Q40" s="84"/>
+      <c r="M40" s="80"/>
+      <c r="N40" s="64"/>
+      <c r="O40" s="64"/>
+      <c r="P40" s="64"/>
+      <c r="Q40" s="61"/>
       <c r="R40" s="6"/>
     </row>
     <row r="41" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="68"/>
+      <c r="A41" s="66"/>
       <c r="B41" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="63"/>
-      <c r="J41" s="63"/>
-      <c r="K41" s="63"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="64"/>
+      <c r="K41" s="64"/>
       <c r="L41" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="M41" s="66"/>
-      <c r="N41" s="63"/>
-      <c r="O41" s="63"/>
-      <c r="P41" s="63"/>
-      <c r="Q41" s="84"/>
+      <c r="M41" s="80"/>
+      <c r="N41" s="64"/>
+      <c r="O41" s="64"/>
+      <c r="P41" s="64"/>
+      <c r="Q41" s="61"/>
       <c r="R41" s="6"/>
     </row>
     <row r="42" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="68"/>
+      <c r="A42" s="66"/>
       <c r="B42" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="63"/>
-      <c r="J42" s="63"/>
-      <c r="K42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="64"/>
       <c r="L42" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="M42" s="66"/>
-      <c r="N42" s="63"/>
-      <c r="O42" s="63"/>
-      <c r="P42" s="63"/>
-      <c r="Q42" s="84"/>
+      <c r="M42" s="80"/>
+      <c r="N42" s="64"/>
+      <c r="O42" s="64"/>
+      <c r="P42" s="64"/>
+      <c r="Q42" s="61"/>
       <c r="R42" s="6"/>
     </row>
     <row r="43" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="68"/>
+      <c r="A43" s="66"/>
       <c r="B43" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
-      <c r="K43" s="63"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="64"/>
+      <c r="K43" s="64"/>
       <c r="L43" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="M43" s="66"/>
-      <c r="N43" s="63"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="63"/>
-      <c r="Q43" s="84"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="64"/>
+      <c r="O43" s="64"/>
+      <c r="P43" s="64"/>
+      <c r="Q43" s="61"/>
       <c r="R43" s="6"/>
     </row>
     <row r="44" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="68"/>
+      <c r="A44" s="66"/>
       <c r="B44" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="63"/>
-      <c r="K44" s="63"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="64"/>
       <c r="L44" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="M44" s="66"/>
-      <c r="N44" s="63"/>
-      <c r="O44" s="63"/>
-      <c r="P44" s="63"/>
-      <c r="Q44" s="84"/>
+      <c r="M44" s="80"/>
+      <c r="N44" s="64"/>
+      <c r="O44" s="64"/>
+      <c r="P44" s="64"/>
+      <c r="Q44" s="61"/>
       <c r="R44" s="40"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="68"/>
+      <c r="A45" s="66"/>
       <c r="B45" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="63"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="64"/>
       <c r="L45" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="M45" s="66"/>
-      <c r="N45" s="63"/>
-      <c r="O45" s="63"/>
-      <c r="P45" s="63"/>
-      <c r="Q45" s="84"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="64"/>
+      <c r="O45" s="64"/>
+      <c r="P45" s="64"/>
+      <c r="Q45" s="61"/>
       <c r="R45" s="6"/>
     </row>
     <row r="46" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="68"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
-      <c r="K46" s="63"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="64"/>
+      <c r="K46" s="64"/>
       <c r="L46" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="M46" s="66"/>
-      <c r="N46" s="63"/>
-      <c r="O46" s="63"/>
-      <c r="P46" s="63"/>
-      <c r="Q46" s="84"/>
+      <c r="M46" s="80"/>
+      <c r="N46" s="64"/>
+      <c r="O46" s="64"/>
+      <c r="P46" s="64"/>
+      <c r="Q46" s="61"/>
       <c r="R46" s="40"/>
     </row>
     <row r="47" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="68"/>
+      <c r="A47" s="66"/>
       <c r="B47" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="63"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="64"/>
       <c r="L47" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="M47" s="66"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="63"/>
-      <c r="P47" s="63"/>
-      <c r="Q47" s="84"/>
+      <c r="M47" s="80"/>
+      <c r="N47" s="64"/>
+      <c r="O47" s="64"/>
+      <c r="P47" s="64"/>
+      <c r="Q47" s="61"/>
       <c r="R47" s="40"/>
     </row>
     <row r="48" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="68"/>
+      <c r="A48" s="66"/>
       <c r="B48" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="C48" s="63"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
-      <c r="G48" s="63"/>
-      <c r="H48" s="63"/>
-      <c r="I48" s="63"/>
-      <c r="J48" s="63"/>
-      <c r="K48" s="63"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+      <c r="K48" s="64"/>
       <c r="L48" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="M48" s="66"/>
-      <c r="N48" s="63"/>
-      <c r="O48" s="63"/>
-      <c r="P48" s="63"/>
-      <c r="Q48" s="84"/>
+      <c r="M48" s="80"/>
+      <c r="N48" s="64"/>
+      <c r="O48" s="64"/>
+      <c r="P48" s="64"/>
+      <c r="Q48" s="61"/>
       <c r="R48" s="40"/>
     </row>
     <row r="49" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="68"/>
+      <c r="A49" s="66"/>
       <c r="B49" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="64"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="64"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="65"/>
+      <c r="J49" s="65"/>
+      <c r="K49" s="65"/>
       <c r="L49" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="M49" s="67"/>
-      <c r="N49" s="64"/>
-      <c r="O49" s="64"/>
-      <c r="P49" s="64"/>
-      <c r="Q49" s="85"/>
+      <c r="M49" s="82"/>
+      <c r="N49" s="65"/>
+      <c r="O49" s="65"/>
+      <c r="P49" s="65"/>
+      <c r="Q49" s="62"/>
       <c r="R49" s="40"/>
     </row>
     <row r="50" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="62" t="s">
+      <c r="A50" s="63" t="s">
         <v>270</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C50" s="83" t="s">
         <v>251</v>
       </c>
-      <c r="D50" s="56" t="s">
+      <c r="D50" s="83" t="s">
         <v>286</v>
       </c>
-      <c r="E50" s="56" t="s">
+      <c r="E50" s="83" t="s">
         <v>255</v>
       </c>
-      <c r="F50" s="56" t="s">
+      <c r="F50" s="83" t="s">
         <v>253</v>
       </c>
-      <c r="G50" s="56" t="s">
+      <c r="G50" s="83" t="s">
         <v>254</v>
       </c>
-      <c r="H50" s="56" t="s">
+      <c r="H50" s="83" t="s">
         <v>252</v>
       </c>
-      <c r="I50" s="56" t="s">
+      <c r="I50" s="83" t="s">
         <v>256</v>
       </c>
-      <c r="J50" s="56" t="s">
+      <c r="J50" s="83" t="s">
         <v>259</v>
       </c>
-      <c r="K50" s="56" t="s">
+      <c r="K50" s="83" t="s">
         <v>260</v>
       </c>
       <c r="L50" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="M50" s="59" t="s">
+      <c r="M50" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="N50" s="56" t="s">
+      <c r="N50" s="83" t="s">
         <v>294</v>
       </c>
-      <c r="O50" s="56"/>
-      <c r="P50" s="56"/>
-      <c r="Q50" s="83" t="s">
+      <c r="O50" s="83"/>
+      <c r="P50" s="83"/>
+      <c r="Q50" s="60" t="s">
         <v>306</v>
       </c>
       <c r="R50" s="40"/>
     </row>
     <row r="51" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="63"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="84"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="84"/>
+      <c r="J51" s="84"/>
+      <c r="K51" s="84"/>
       <c r="L51" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="M51" s="60"/>
-      <c r="N51" s="57"/>
-      <c r="O51" s="57"/>
-      <c r="P51" s="57"/>
-      <c r="Q51" s="84"/>
+      <c r="M51" s="87"/>
+      <c r="N51" s="84"/>
+      <c r="O51" s="84"/>
+      <c r="P51" s="84"/>
+      <c r="Q51" s="61"/>
       <c r="R51" s="40"/>
     </row>
     <row r="52" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="63"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
+      <c r="C52" s="84"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="84"/>
+      <c r="G52" s="84"/>
+      <c r="H52" s="84"/>
+      <c r="I52" s="84"/>
+      <c r="J52" s="84"/>
+      <c r="K52" s="84"/>
       <c r="L52" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="M52" s="60"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
-      <c r="P52" s="57"/>
-      <c r="Q52" s="84"/>
+      <c r="M52" s="87"/>
+      <c r="N52" s="84"/>
+      <c r="O52" s="84"/>
+      <c r="P52" s="84"/>
+      <c r="Q52" s="61"/>
       <c r="R52" s="40"/>
     </row>
     <row r="53" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="64"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="58"/>
-      <c r="K53" s="58"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="85"/>
+      <c r="I53" s="85"/>
+      <c r="J53" s="85"/>
+      <c r="K53" s="85"/>
       <c r="L53" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="M53" s="61"/>
-      <c r="N53" s="58"/>
-      <c r="O53" s="58"/>
-      <c r="P53" s="58"/>
-      <c r="Q53" s="85"/>
+      <c r="M53" s="88"/>
+      <c r="N53" s="85"/>
+      <c r="O53" s="85"/>
+      <c r="P53" s="85"/>
+      <c r="Q53" s="62"/>
       <c r="R53" s="40"/>
     </row>
     <row r="54" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4223,7 +4232,7 @@
       <c r="N54" s="37"/>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
-      <c r="Q54" s="86"/>
+      <c r="Q54" s="57"/>
       <c r="R54" s="40"/>
     </row>
     <row r="55" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4247,7 +4256,7 @@
       <c r="N55" s="37"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
-      <c r="Q55" s="87"/>
+      <c r="Q55" s="58"/>
       <c r="R55" s="40"/>
     </row>
     <row r="56" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4271,7 +4280,7 @@
       <c r="N56" s="41"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
-      <c r="Q56" s="86"/>
+      <c r="Q56" s="57"/>
       <c r="R56" s="6"/>
     </row>
     <row r="57" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4295,7 +4304,7 @@
       <c r="N57" s="42"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
-      <c r="Q57" s="86"/>
+      <c r="Q57" s="57"/>
       <c r="R57" s="6"/>
     </row>
     <row r="58" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4319,7 +4328,7 @@
       <c r="N58" s="42"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
-      <c r="Q58" s="87"/>
+      <c r="Q58" s="58"/>
       <c r="R58" s="6"/>
     </row>
     <row r="59" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4343,7 +4352,7 @@
       <c r="N59" s="42"/>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
-      <c r="Q59" s="87"/>
+      <c r="Q59" s="58"/>
       <c r="R59" s="6"/>
     </row>
     <row r="60" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4367,7 +4376,7 @@
       <c r="N60" s="42"/>
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
-      <c r="Q60" s="86"/>
+      <c r="Q60" s="57"/>
       <c r="R60" s="6"/>
     </row>
     <row r="61" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -4391,7 +4400,7 @@
       <c r="N61" s="42"/>
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
-      <c r="Q61" s="88"/>
+      <c r="Q61" s="59"/>
       <c r="R61" s="6"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
@@ -6836,12 +6845,75 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="Q50:Q53"/>
-    <mergeCell ref="Q36:Q49"/>
-    <mergeCell ref="Q4:Q12"/>
-    <mergeCell ref="Q13:Q20"/>
-    <mergeCell ref="Q21:Q25"/>
-    <mergeCell ref="Q28:Q35"/>
+    <mergeCell ref="H50:H53"/>
+    <mergeCell ref="I50:I53"/>
+    <mergeCell ref="P50:P53"/>
+    <mergeCell ref="O50:O53"/>
+    <mergeCell ref="J50:J53"/>
+    <mergeCell ref="K50:K53"/>
+    <mergeCell ref="M50:M53"/>
+    <mergeCell ref="N50:N53"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="M36:M49"/>
+    <mergeCell ref="N36:N49"/>
+    <mergeCell ref="D36:D49"/>
+    <mergeCell ref="E36:E49"/>
+    <mergeCell ref="F36:F49"/>
+    <mergeCell ref="G36:G49"/>
+    <mergeCell ref="I36:I49"/>
+    <mergeCell ref="J36:J49"/>
+    <mergeCell ref="K36:K49"/>
+    <mergeCell ref="A36:A49"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="F50:F53"/>
+    <mergeCell ref="G50:G53"/>
+    <mergeCell ref="O36:O49"/>
+    <mergeCell ref="P36:P49"/>
+    <mergeCell ref="M21:M25"/>
+    <mergeCell ref="N21:N25"/>
+    <mergeCell ref="O21:O25"/>
+    <mergeCell ref="P21:P25"/>
+    <mergeCell ref="M28:M35"/>
+    <mergeCell ref="N28:N35"/>
+    <mergeCell ref="O28:O35"/>
+    <mergeCell ref="P28:P35"/>
+    <mergeCell ref="M4:M12"/>
+    <mergeCell ref="N4:N12"/>
+    <mergeCell ref="O4:O12"/>
+    <mergeCell ref="P4:P12"/>
+    <mergeCell ref="K13:K20"/>
+    <mergeCell ref="M13:M20"/>
+    <mergeCell ref="N13:N20"/>
+    <mergeCell ref="O13:O20"/>
+    <mergeCell ref="P13:P20"/>
+    <mergeCell ref="K4:K12"/>
+    <mergeCell ref="J28:J35"/>
+    <mergeCell ref="K28:K35"/>
+    <mergeCell ref="H28:H35"/>
+    <mergeCell ref="H36:H49"/>
+    <mergeCell ref="E4:E12"/>
+    <mergeCell ref="E28:E35"/>
+    <mergeCell ref="F28:F35"/>
+    <mergeCell ref="G28:G35"/>
+    <mergeCell ref="I28:I35"/>
+    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="G21:G25"/>
+    <mergeCell ref="J4:J12"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="D4:D12"/>
+    <mergeCell ref="F4:F12"/>
+    <mergeCell ref="G4:G12"/>
+    <mergeCell ref="D13:D20"/>
+    <mergeCell ref="E13:E20"/>
+    <mergeCell ref="F13:F20"/>
+    <mergeCell ref="G13:G20"/>
+    <mergeCell ref="D28:D35"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C28:C35"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="C13:C20"/>
     <mergeCell ref="C36:C49"/>
     <mergeCell ref="D21:D25"/>
     <mergeCell ref="E21:E25"/>
@@ -6858,75 +6930,12 @@
     <mergeCell ref="J21:J25"/>
     <mergeCell ref="K21:K25"/>
     <mergeCell ref="I4:I12"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="D4:D12"/>
-    <mergeCell ref="F4:F12"/>
-    <mergeCell ref="G4:G12"/>
-    <mergeCell ref="D13:D20"/>
-    <mergeCell ref="E13:E20"/>
-    <mergeCell ref="F13:F20"/>
-    <mergeCell ref="G13:G20"/>
-    <mergeCell ref="D28:D35"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C28:C35"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="C13:C20"/>
-    <mergeCell ref="J28:J35"/>
-    <mergeCell ref="K28:K35"/>
-    <mergeCell ref="H28:H35"/>
-    <mergeCell ref="H36:H49"/>
-    <mergeCell ref="E4:E12"/>
-    <mergeCell ref="E28:E35"/>
-    <mergeCell ref="F28:F35"/>
-    <mergeCell ref="G28:G35"/>
-    <mergeCell ref="I28:I35"/>
-    <mergeCell ref="F21:F25"/>
-    <mergeCell ref="G21:G25"/>
-    <mergeCell ref="J4:J12"/>
-    <mergeCell ref="M4:M12"/>
-    <mergeCell ref="N4:N12"/>
-    <mergeCell ref="O4:O12"/>
-    <mergeCell ref="P4:P12"/>
-    <mergeCell ref="K13:K20"/>
-    <mergeCell ref="M13:M20"/>
-    <mergeCell ref="N13:N20"/>
-    <mergeCell ref="O13:O20"/>
-    <mergeCell ref="P13:P20"/>
-    <mergeCell ref="K4:K12"/>
-    <mergeCell ref="O36:O49"/>
-    <mergeCell ref="P36:P49"/>
-    <mergeCell ref="M21:M25"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="M28:M35"/>
-    <mergeCell ref="N28:N35"/>
-    <mergeCell ref="O28:O35"/>
-    <mergeCell ref="P28:P35"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="M36:M49"/>
-    <mergeCell ref="N36:N49"/>
-    <mergeCell ref="D36:D49"/>
-    <mergeCell ref="E36:E49"/>
-    <mergeCell ref="F36:F49"/>
-    <mergeCell ref="G36:G49"/>
-    <mergeCell ref="I36:I49"/>
-    <mergeCell ref="J36:J49"/>
-    <mergeCell ref="K36:K49"/>
-    <mergeCell ref="A36:A49"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="F50:F53"/>
-    <mergeCell ref="G50:G53"/>
-    <mergeCell ref="H50:H53"/>
-    <mergeCell ref="I50:I53"/>
-    <mergeCell ref="P50:P53"/>
-    <mergeCell ref="O50:O53"/>
-    <mergeCell ref="J50:J53"/>
-    <mergeCell ref="K50:K53"/>
-    <mergeCell ref="M50:M53"/>
-    <mergeCell ref="N50:N53"/>
+    <mergeCell ref="Q50:Q53"/>
+    <mergeCell ref="Q36:Q49"/>
+    <mergeCell ref="Q4:Q12"/>
+    <mergeCell ref="Q13:Q20"/>
+    <mergeCell ref="Q21:Q25"/>
+    <mergeCell ref="Q28:Q35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1"/>

</xml_diff>